<commit_message>
fixed rounding issues, estimation flow and naming, receipt form post upload. added data for more diets
</commit_message>
<xml_diff>
--- a/app/datasets/berners-leeFootprintOfFood.xlsx
+++ b/app/datasets/berners-leeFootprintOfFood.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="339" documentId="8_{D00D6C2E-171F-4325-A77C-E1B876CC46D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BAA2DB8-5937-4F33-A6A8-A8721C1ECAD8}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="21240" windowHeight="20985" xr2:uid="{037CA489-A1BD-4E7F-AC07-F181B0C46B24}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{037CA489-A1BD-4E7F-AC07-F181B0C46B24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2793F6F-C4E5-470C-BD0B-6ED6ACA87019}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
       <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>

</xml_diff>